<commit_message>
more options for tweaking sigmas etc
</commit_message>
<xml_diff>
--- a/docs/Examples/Diad_Fitting_Nov22nd2022/strong_Diads.xlsx
+++ b/docs/Examples/Diad_Fitting_Nov22nd2022/strong_Diads.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>filename</t>
   </si>
@@ -79,6 +79,27 @@
     <t>Diad2_fwhm</t>
   </si>
   <si>
+    <t>Diad2_refit</t>
+  </si>
+  <si>
+    <t>HB1_Cent</t>
+  </si>
+  <si>
+    <t>HB1_Area</t>
+  </si>
+  <si>
+    <t>HB2_Cent</t>
+  </si>
+  <si>
+    <t>HB2_Area</t>
+  </si>
+  <si>
+    <t>C13_Cent</t>
+  </si>
+  <si>
+    <t>C13_Area</t>
+  </si>
+  <si>
     <t>POC8</t>
   </si>
   <si>
@@ -101,6 +122,12 @@
   </si>
   <si>
     <t>POC3</t>
+  </si>
+  <si>
+    <t>Flagged Warnings:</t>
+  </si>
+  <si>
+    <t>Flagged Warnings: G_HighAmp</t>
   </si>
 </sst>
 </file>
@@ -458,13 +485,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:AC9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:29">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,43 +555,64 @@
       <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:29">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C2">
-        <v>104.4425746990862</v>
+        <v>104.4416826061054</v>
       </c>
       <c r="D2">
-        <v>1282.730868820775</v>
+        <v>1282.731560903755</v>
       </c>
       <c r="E2">
-        <v>14906.39371105165</v>
+        <v>14938.35919160645</v>
       </c>
       <c r="F2">
-        <v>1282.730718813274</v>
+        <v>1282.731610906255</v>
       </c>
       <c r="G2">
-        <v>44947.63800973798</v>
+        <v>46056.9278321534</v>
       </c>
       <c r="H2">
-        <v>1.10702453768404</v>
+        <v>1.10685943665716</v>
       </c>
       <c r="J2">
-        <v>18.49878234783836</v>
+        <v>26.05434347263179</v>
       </c>
       <c r="K2">
-        <v>0.6927723515641337</v>
+        <v>0.7347758307474805</v>
       </c>
       <c r="L2">
-        <v>2.214049075368081</v>
-      </c>
-      <c r="M2" t="b">
-        <v>0</v>
+        <v>2.21371887331432</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
       </c>
       <c r="N2">
         <v>1387.17314350486</v>
@@ -590,43 +638,64 @@
       <c r="V2">
         <v>1.956354341044958</v>
       </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2">
+        <v>1262.700591628001</v>
+      </c>
+      <c r="Y2">
+        <v>6502.745849278953</v>
+      </c>
+      <c r="Z2">
+        <v>1408.426449771047</v>
+      </c>
+      <c r="AA2">
+        <v>9658.957575289749</v>
+      </c>
+      <c r="AB2">
+        <v>1369.639259871846</v>
+      </c>
+      <c r="AC2">
+        <v>1270.251510690677</v>
+      </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:29">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C3">
-        <v>104.9481986106382</v>
+        <v>104.9482015439476</v>
       </c>
       <c r="D3">
-        <v>1281.782461697167</v>
+        <v>1281.782458763857</v>
       </c>
       <c r="E3">
-        <v>19888.94515174412</v>
+        <v>19888.96018268805</v>
       </c>
       <c r="F3">
-        <v>1281.782411694667</v>
+        <v>1281.782408761357</v>
       </c>
       <c r="G3">
-        <v>59001.91880459722</v>
+        <v>59002.26018971133</v>
       </c>
       <c r="H3">
-        <v>1.071728699732787</v>
+        <v>1.071727856268716</v>
       </c>
       <c r="J3">
-        <v>27.54146420985196</v>
+        <v>27.54772052758774</v>
       </c>
       <c r="K3">
-        <v>0.7429136612205511</v>
+        <v>0.7429253089663556</v>
       </c>
       <c r="L3">
-        <v>2.143457399465574</v>
-      </c>
-      <c r="M3" t="b">
-        <v>0</v>
+        <v>2.143455712537432</v>
+      </c>
+      <c r="M3" t="s">
+        <v>36</v>
       </c>
       <c r="N3">
         <v>1386.730660307805</v>
@@ -652,43 +721,64 @@
       <c r="V3">
         <v>2.06375947820929</v>
       </c>
+      <c r="W3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3">
+        <v>1261.760446403409</v>
+      </c>
+      <c r="Y3">
+        <v>8678.348275501039</v>
+      </c>
+      <c r="Z3">
+        <v>1408.059745170119</v>
+      </c>
+      <c r="AA3">
+        <v>10528.49189397234</v>
+      </c>
+      <c r="AB3">
+        <v>1369.532303367029</v>
+      </c>
+      <c r="AC3">
+        <v>1329.214833356688</v>
+      </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:29">
       <c r="A4" s="1">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C4">
-        <v>104.5378114030855</v>
+        <v>104.5284597401205</v>
       </c>
       <c r="D4">
-        <v>1282.549917620856</v>
+        <v>1282.556569148814</v>
       </c>
       <c r="E4">
-        <v>26125.69411200816</v>
+        <v>26070.74957900919</v>
       </c>
       <c r="F4">
-        <v>1282.547067478349</v>
+        <v>1282.556419141314</v>
       </c>
       <c r="G4">
-        <v>77936.44893853911</v>
+        <v>77582.4028390746</v>
       </c>
       <c r="H4">
-        <v>1.0898720731134</v>
+        <v>1.096548351424453</v>
       </c>
       <c r="J4">
-        <v>47.50709129768414</v>
+        <v>36.40482454093567</v>
       </c>
       <c r="K4">
-        <v>0.7108862664864701</v>
+        <v>0.6874518354469279</v>
       </c>
       <c r="L4">
-        <v>2.179744146226799</v>
-      </c>
-      <c r="M4" t="b">
-        <v>1</v>
+        <v>2.193096702848907</v>
+      </c>
+      <c r="M4" t="s">
+        <v>36</v>
       </c>
       <c r="N4">
         <v>1387.084928883934</v>
@@ -714,43 +804,64 @@
       <c r="V4">
         <v>1.983923474782245</v>
       </c>
+      <c r="W4" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4">
+        <v>1262.500374127099</v>
+      </c>
+      <c r="Y4">
+        <v>11118.86746785118</v>
+      </c>
+      <c r="Z4">
+        <v>1408.440059140436</v>
+      </c>
+      <c r="AA4">
+        <v>14245.34123706916</v>
+      </c>
+      <c r="AB4">
+        <v>1369.606721625361</v>
+      </c>
+      <c r="AC4">
+        <v>1726.645932763279</v>
+      </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:29">
       <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C5">
-        <v>104.5928468061729</v>
+        <v>104.5928477781515</v>
       </c>
       <c r="D5">
-        <v>1282.422381017461</v>
+        <v>1282.422380045482</v>
       </c>
       <c r="E5">
-        <v>27783.20867138372</v>
+        <v>27783.21832541282</v>
       </c>
       <c r="F5">
-        <v>1282.422231009961</v>
+        <v>1282.422230037982</v>
       </c>
       <c r="G5">
-        <v>82189.03412892266</v>
+        <v>82189.29412392301</v>
       </c>
       <c r="H5">
-        <v>1.086462528188054</v>
+        <v>1.086462323972746</v>
       </c>
       <c r="J5">
-        <v>33.2358927304521</v>
+        <v>33.23821993934605</v>
       </c>
       <c r="K5">
-        <v>0.6975662738323346</v>
+        <v>0.6975720889834258</v>
       </c>
       <c r="L5">
-        <v>2.172925056376108</v>
-      </c>
-      <c r="M5" t="b">
-        <v>0</v>
+        <v>2.172924647945491</v>
+      </c>
+      <c r="M5" t="s">
+        <v>36</v>
       </c>
       <c r="N5">
         <v>1387.015127818634</v>
@@ -776,43 +887,64 @@
       <c r="V5">
         <v>1.99784212500284</v>
       </c>
+      <c r="W5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5">
+        <v>1262.422595420142</v>
+      </c>
+      <c r="Y5">
+        <v>12082.02179617755</v>
+      </c>
+      <c r="Z5">
+        <v>1408.403012072601</v>
+      </c>
+      <c r="AA5">
+        <v>7959.804678916306</v>
+      </c>
+      <c r="AB5">
+        <v>1370.524840691275</v>
+      </c>
+      <c r="AC5">
+        <v>631.2480053987308</v>
+      </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:29">
       <c r="A6" s="1">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>104.6487359290154</v>
+        <v>104.6494847777587</v>
       </c>
       <c r="D6">
-        <v>1282.315324617347</v>
+        <v>1282.314775778605</v>
       </c>
       <c r="E6">
-        <v>28729.21125653609</v>
+        <v>28640.20313606597</v>
       </c>
       <c r="F6">
-        <v>1282.315374619847</v>
+        <v>1282.314625771104</v>
       </c>
       <c r="G6">
-        <v>87787.2242002834</v>
+        <v>84494.64331070393</v>
       </c>
       <c r="H6">
-        <v>1.082845221236768</v>
+        <v>1.082228038054093</v>
       </c>
       <c r="J6">
-        <v>57.28451394872647</v>
+        <v>35.00185500506925</v>
       </c>
       <c r="K6">
-        <v>0.7652797283714029</v>
+        <v>0.7019658137253</v>
       </c>
       <c r="L6">
-        <v>2.165690442473536</v>
-      </c>
-      <c r="M6" t="b">
-        <v>1</v>
+        <v>2.164456076108186</v>
+      </c>
+      <c r="M6" t="s">
+        <v>36</v>
       </c>
       <c r="N6">
         <v>1386.964160551363</v>
@@ -838,43 +970,64 @@
       <c r="V6">
         <v>2.007801008849404</v>
       </c>
+      <c r="W6" t="s">
+        <v>36</v>
+      </c>
+      <c r="X6">
+        <v>1262.267393849275</v>
+      </c>
+      <c r="Y6">
+        <v>12397.33240083351</v>
+      </c>
+      <c r="Z6">
+        <v>1408.307848334188</v>
+      </c>
+      <c r="AA6">
+        <v>15510.18480839576</v>
+      </c>
+      <c r="AB6">
+        <v>1369.588992614416</v>
+      </c>
+      <c r="AC6">
+        <v>1909.746848901286</v>
+      </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:29">
       <c r="A7" s="1">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C7">
-        <v>104.7006076909645</v>
+        <v>104.7006071670767</v>
       </c>
       <c r="D7">
-        <v>1282.221380320299</v>
+        <v>1282.221380844187</v>
       </c>
       <c r="E7">
-        <v>28849.95166788357</v>
+        <v>28849.94416119181</v>
       </c>
       <c r="F7">
-        <v>1282.221330317799</v>
+        <v>1282.221330841687</v>
       </c>
       <c r="G7">
-        <v>84972.86807868385</v>
+        <v>84972.64515497365</v>
       </c>
       <c r="H7">
-        <v>1.075852099807332</v>
+        <v>1.075852168341284</v>
       </c>
       <c r="J7">
-        <v>35.13569201322791</v>
+        <v>35.13331555840349</v>
       </c>
       <c r="K7">
-        <v>0.712122562219541</v>
+        <v>0.7121180399087974</v>
       </c>
       <c r="L7">
-        <v>2.151704199614664</v>
-      </c>
-      <c r="M7" t="b">
-        <v>0</v>
+        <v>2.151704336682569</v>
+      </c>
+      <c r="M7" t="s">
+        <v>36</v>
       </c>
       <c r="N7">
         <v>1386.921988011264</v>
@@ -900,43 +1053,64 @@
       <c r="V7">
         <v>2.021408254455575</v>
       </c>
+      <c r="W7" t="s">
+        <v>36</v>
+      </c>
+      <c r="X7">
+        <v>1262.172418639208</v>
+      </c>
+      <c r="Y7">
+        <v>12246.49910889012</v>
+      </c>
+      <c r="Z7">
+        <v>1408.259277165743</v>
+      </c>
+      <c r="AA7">
+        <v>16029.08321640206</v>
+      </c>
+      <c r="AB7">
+        <v>1369.568946009335</v>
+      </c>
+      <c r="AC7">
+        <v>1853.023849203802</v>
+      </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:29">
       <c r="A8" s="1">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C8">
-        <v>104.8871729540144</v>
+        <v>104.8871737837685</v>
       </c>
       <c r="D8">
-        <v>1281.888682685162</v>
+        <v>1281.888681855408</v>
       </c>
       <c r="E8">
-        <v>30295.70183096123</v>
+        <v>30295.70622960277</v>
       </c>
       <c r="F8">
-        <v>1281.888532677662</v>
+        <v>1281.888531847908</v>
       </c>
       <c r="G8">
-        <v>89463.15198056828</v>
+        <v>89463.14199920882</v>
       </c>
       <c r="H8">
-        <v>1.071076413346379</v>
+        <v>1.071075902070278</v>
       </c>
       <c r="J8">
-        <v>39.42431652554543</v>
+        <v>39.4268050741318</v>
       </c>
       <c r="K8">
-        <v>0.7332669497009476</v>
+        <v>0.733267951110507</v>
       </c>
       <c r="L8">
-        <v>2.142152826692758</v>
-      </c>
-      <c r="M8" t="b">
-        <v>0</v>
+        <v>2.142151804140556</v>
+      </c>
+      <c r="M8" t="s">
+        <v>36</v>
       </c>
       <c r="N8">
         <v>1386.775755634176</v>
@@ -962,43 +1136,64 @@
       <c r="V8">
         <v>2.052743945666267</v>
       </c>
+      <c r="W8" t="s">
+        <v>36</v>
+      </c>
+      <c r="X8">
+        <v>1261.867346691758</v>
+      </c>
+      <c r="Y8">
+        <v>13265.06820181278</v>
+      </c>
+      <c r="Z8">
+        <v>1408.092802551151</v>
+      </c>
+      <c r="AA8">
+        <v>16137.34347282708</v>
+      </c>
+      <c r="AB8">
+        <v>1369.543265961725</v>
+      </c>
+      <c r="AC8">
+        <v>2004.488423201079</v>
+      </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:29">
       <c r="A9" s="1">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C9">
-        <v>104.80945106739</v>
+        <v>104.8021260425749</v>
       </c>
       <c r="D9">
-        <v>1282.031124675205</v>
+        <v>1282.036649610016</v>
       </c>
       <c r="E9">
-        <v>29858.49283846282</v>
+        <v>29796.23314190377</v>
       </c>
       <c r="F9">
-        <v>1282.0291745777</v>
+        <v>1282.036499602515</v>
       </c>
       <c r="G9">
-        <v>89472.55024240245</v>
+        <v>87724.00063667075</v>
       </c>
       <c r="H9">
-        <v>1.071501073374309</v>
+        <v>1.073059888351807</v>
       </c>
       <c r="J9">
-        <v>57.15751791713139</v>
+        <v>38.25837991113856</v>
       </c>
       <c r="K9">
-        <v>0.753990971408187</v>
+        <v>0.7205048029720834</v>
       </c>
       <c r="L9">
-        <v>2.143002146748618</v>
-      </c>
-      <c r="M9" t="b">
-        <v>1</v>
+        <v>2.146119776703614</v>
+      </c>
+      <c r="M9" t="s">
+        <v>36</v>
       </c>
       <c r="N9">
         <v>1386.83867564759</v>
@@ -1023,6 +1218,27 @@
       </c>
       <c r="V9">
         <v>2.042717718221378</v>
+      </c>
+      <c r="W9" t="s">
+        <v>36</v>
+      </c>
+      <c r="X9">
+        <v>1262.019647960024</v>
+      </c>
+      <c r="Y9">
+        <v>12918.63043263268</v>
+      </c>
+      <c r="Z9">
+        <v>1408.182013521922</v>
+      </c>
+      <c r="AA9">
+        <v>15827.56809427078</v>
+      </c>
+      <c r="AB9">
+        <v>1369.550184344768</v>
+      </c>
+      <c r="AC9">
+        <v>1955.040423331327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>